<commit_message>
Add Installation pass-through and image handling: pass Installation to renderer, normalize images to data-URIs, include image field when adding products, and helper scripts for inspection/preview
</commit_message>
<xml_diff>
--- a/data/logs.xlsx
+++ b/data/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-28 12:10:02</t>
+          <t>2025-12-07 23:55:36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -490,7 +490,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-11-28 12:10:02</t>
+          <t>2025-12-07 23:55:36</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -517,7 +517,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-11-28 12:10:03</t>
+          <t>2025-12-07 23:55:37</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-11-28 12:10:03</t>
+          <t>2025-12-07 23:55:37</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -554,24 +554,24 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Quotation</t>
+          <t>quotation</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>quotation_created</t>
+          <t>access_granted</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Client: Fahaf, Amount: 3300.0</t>
+          <t>Opened quotation page</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-11-28 12:19:59</t>
+          <t>2025-12-07 23:55:40</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -598,7 +598,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-11-28 12:19:59</t>
+          <t>2025-12-07 23:55:42</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -608,24 +608,24 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Quotation</t>
+          <t>quotation</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>quotation_created</t>
+          <t>access_granted</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Client: Fahaf, Amount: 3300.0</t>
+          <t>Opened quotation page</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-11-28 12:21:41</t>
+          <t>2025-12-07 23:55:44</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-11-28 12:21:49</t>
+          <t>2025-12-07 23:56:08</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>reports</t>
+          <t>settings</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -672,14 +672,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Opened reports page</t>
+          <t>Opened settings page</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-11-28 12:21:52</t>
+          <t>2025-12-07 23:56:11</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -689,17 +689,1529 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:56:13</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>products</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:56:18</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:56:18</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:56:24</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:56:26</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:56:26</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:56:28</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:56:30</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:56:31</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:59:35</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:59:35</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:59:37</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:59:41</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:59:42</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:59:42</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:59:42</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:59:44</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:59:45</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:59:53</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:59:55</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:59:55</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:59:56</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-12-07 23:59:58</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:00:26</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:00:29</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:00:29</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:00:32</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:00:32</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:00:34</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:00:34</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:00:35</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:00:36</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:00:36</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:00:37</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:00:53</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:00:57</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:00:59</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:01:00</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:05:01</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:05:01</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:05:04</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:05:12</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:05:15</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:05:15</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:05:15</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:05:17</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:05:18</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:06:07</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:06:07</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:06:09</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:06:13</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:06:14</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:06:16</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:06:16</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:06:18</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2025-12-08 00:06:19</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add database connection utilities and import scripts for products and customers
</commit_message>
<xml_diff>
--- a/data/logs.xlsx
+++ b/data/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E225"/>
+  <dimension ref="A1:E286"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6508,6 +6508,1653 @@
         </is>
       </c>
     </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:26:12</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:26:12</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:26:14</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:34:16</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:34:16</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:34:18</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:34:22</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:34:25</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:36:13</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:36:13</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:36:15</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:44:04</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:44:04</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:45:24</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:45:24</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:48:07</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>receipt</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>Opened receipt page</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:48:08</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>customers</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>Opened customers page</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:48:09</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:48:10</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:48:21</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>settings</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>Opened settings page</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:55:13</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:55:13</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:55:15</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:55:16</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:55:17</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:55:46</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:55:50</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>receipt</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>Opened receipt page</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:55:51</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>customers</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>Opened customers page</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:55:53</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>settings</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>Opened settings page</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:56:08</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:56:13</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:56:19</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:57:02</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:57:09</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:57:15</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:57:22</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>2025-12-08 04:57:29</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:15:42</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:15:42</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:15:45</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:15:46</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:15:50</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:15:52</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:20:59</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:21:03</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:22:12</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:22:13</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:28:44</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:28:44</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:28:46</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:28:47</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:28:51</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:28:52</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:30:39</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:30:39</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:30:49</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>settings</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>Opened settings page</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:30:53</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:30:55</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:30:55</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:30:56</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:30:59</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor system configuration section for improved readability and functionality
</commit_message>
<xml_diff>
--- a/data/logs.xlsx
+++ b/data/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E286"/>
+  <dimension ref="A1:E292"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8155,6 +8155,168 @@
         </is>
       </c>
     </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:50:56</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:50:57</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:50:59</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>settings</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>Opened settings page</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:51:09</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>settings</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>Opened settings page</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:51:13</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>settings</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>Opened settings page</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>2025-12-08 05:51:16</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>settings</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>Opened settings page</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>